<commit_message>
updated readmes and Excel
</commit_message>
<xml_diff>
--- a/SP_2018_03_06_CarToCarCommunicationRECENTST.xlsx
+++ b/SP_2018_03_06_CarToCarCommunicationRECENTST.xlsx
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="135">
   <si>
     <t>startdatum</t>
   </si>
@@ -332,18 +332,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>Correction</t>
-  </si>
-  <si>
-    <t>Poster</t>
-  </si>
-  <si>
-    <t>Presentation</t>
-  </si>
-  <si>
-    <t>Paperwork</t>
-  </si>
-  <si>
     <t>extreme fine tuning</t>
   </si>
   <si>
@@ -416,21 +404,9 @@
     <t>Lasercutting</t>
   </si>
   <si>
-    <t>Week9(25/04/2018)</t>
-  </si>
-  <si>
     <t>Report9</t>
   </si>
   <si>
-    <t>Poster+ideaFormulation</t>
-  </si>
-  <si>
-    <t>Lasercutter</t>
-  </si>
-  <si>
-    <t>SoftwareUpdates</t>
-  </si>
-  <si>
     <t>Inrushcurrent</t>
   </si>
   <si>
@@ -539,17 +515,77 @@
     <t>U</t>
   </si>
   <si>
-    <t>7-Gauthier de Borrekens_poster_ideas</t>
-  </si>
-  <si>
-    <t>7-Asif Wasefi_poster_ideas</t>
+    <t>Report7</t>
+  </si>
+  <si>
+    <t>7-Ali Amir_Lasercutter</t>
+  </si>
+  <si>
+    <t>7-Satish Singh_Poster+ideaFormulation</t>
+  </si>
+  <si>
+    <t>7-Gauthier de Borrekens_SoftwareUpdates</t>
+  </si>
+  <si>
+    <t>7-Daniel Smetankin_Inrushcurrent</t>
+  </si>
+  <si>
+    <t>8-Gauthier de Borrekens_poster_ideas</t>
+  </si>
+  <si>
+    <t>8-Asif Wasefi_poster_ideas</t>
+  </si>
+  <si>
+    <t>8-Daniel Smetankin_poster_design</t>
+  </si>
+  <si>
+    <t>There were a few documents needed to be corrected. For example converting to PDF, deleting tekst in Dutch, using the right template, … Not all the needed tasks have been done as of 09/05/2018. This task shall be delayed until next week.</t>
+  </si>
+  <si>
+    <t>Practical work which was completed by Satish and Ali</t>
+  </si>
+  <si>
+    <t>Week4(21/03/2018)</t>
+  </si>
+  <si>
+    <t>Week5(28/03/2018)</t>
+  </si>
+  <si>
+    <t>Report4</t>
+  </si>
+  <si>
+    <t>Report5</t>
+  </si>
+  <si>
+    <t>Report6</t>
+  </si>
+  <si>
+    <t>Report8</t>
+  </si>
+  <si>
+    <t>There is a pdf, which seems like a preparation. But there is no report of this date.</t>
+  </si>
+  <si>
+    <t>Week6(18/04/2018)</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>Week7(18/04/2018)</t>
+  </si>
+  <si>
+    <t>Week8(02/05/2018)</t>
+  </si>
+  <si>
+    <t>Week9(09/05/2018)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -628,15 +664,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -664,6 +693,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -798,7 +833,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -901,7 +936,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -930,6 +964,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1240,10 +1279,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P77"/>
+  <dimension ref="B1:P78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O71" sqref="O71"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,27 +1301,27 @@
     <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.7109375" customWidth="1"/>
     <col min="15" max="15" width="60.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="34.7109375" customWidth="1"/>
+    <col min="16" max="16" width="85.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="31"/>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
       <c r="P2" s="32"/>
     </row>
     <row r="3" spans="2:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1302,27 +1341,27 @@
     </row>
     <row r="4" spans="2:16" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="26"/>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="51"/>
+      <c r="D4" s="50"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="50" t="s">
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
       <c r="L4" s="19"/>
-      <c r="M4" s="49" t="s">
+      <c r="M4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="49"/>
-      <c r="O4" s="49"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
       <c r="P4" s="20" t="s">
         <v>15</v>
       </c>
@@ -1345,28 +1384,28 @@
       <c r="P5" s="7"/>
     </row>
     <row r="6" spans="2:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="46" t="s">
+      <c r="F6" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="47" t="s">
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
       <c r="L6" s="18"/>
-      <c r="M6" s="48" t="s">
+      <c r="M6" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="48"/>
-      <c r="O6" s="48"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
       <c r="P6" s="28"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
@@ -1472,7 +1511,7 @@
       <c r="M10" s="40"/>
       <c r="N10" s="40"/>
       <c r="O10" s="40" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
@@ -1506,7 +1545,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="40"/>
       <c r="O11" s="40" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
@@ -1540,9 +1579,9 @@
       <c r="M12" s="2"/>
       <c r="N12" s="40"/>
       <c r="O12" s="40" t="s">
-        <v>112</v>
-      </c>
-      <c r="P12" s="44"/>
+        <v>104</v>
+      </c>
+      <c r="P12" s="52"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="25">
@@ -1575,7 +1614,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="40"/>
       <c r="O13" s="40" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
@@ -1676,7 +1715,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="40"/>
       <c r="O17" s="40" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
@@ -1711,7 +1750,7 @@
       <c r="M18" s="40"/>
       <c r="N18" s="40"/>
       <c r="O18" s="40" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
@@ -1746,7 +1785,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="40"/>
       <c r="O19" s="40" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
@@ -1781,7 +1820,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="40"/>
       <c r="O20" s="40" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
@@ -1816,7 +1855,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="40"/>
       <c r="O21" s="40" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
@@ -1866,7 +1905,7 @@
         <v>43173</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="I24" s="39">
         <v>43166</v>
@@ -1880,7 +1919,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="40"/>
       <c r="O24" s="40" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
@@ -1914,9 +1953,9 @@
       <c r="M25" s="2"/>
       <c r="N25" s="40"/>
       <c r="O25" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="P25" s="44"/>
+        <v>106</v>
+      </c>
+      <c r="P25" s="52"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="25">
@@ -1949,7 +1988,7 @@
       <c r="M26" s="40"/>
       <c r="N26" s="40"/>
       <c r="O26" s="40" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
@@ -1982,10 +2021,10 @@
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="40" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="O27" s="40" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
@@ -2020,7 +2059,7 @@
       <c r="M28" s="2"/>
       <c r="N28" s="14"/>
       <c r="O28" s="40" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
@@ -2060,7 +2099,7 @@
         <v>33</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E31" s="16" t="s">
         <v>13</v>
@@ -2087,7 +2126,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="38"/>
       <c r="O31" s="40" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
@@ -2095,7 +2134,7 @@
         <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E32" s="16" t="s">
         <v>13</v>
@@ -2107,7 +2146,7 @@
         <v>43180</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="I32" s="39">
         <v>43173</v>
@@ -2122,7 +2161,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="38"/>
       <c r="O32" s="40" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
@@ -2130,7 +2169,7 @@
         <v>35</v>
       </c>
       <c r="D33" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E33" s="16" t="s">
         <v>13</v>
@@ -2142,7 +2181,7 @@
         <v>43180</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="I33" s="39">
         <v>43173</v>
@@ -2157,12 +2196,12 @@
       <c r="M33" s="2"/>
       <c r="N33" s="14"/>
       <c r="O33" s="40" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E34" s="16" t="s">
         <v>13</v>
@@ -2189,16 +2228,16 @@
       <c r="M34" s="40"/>
       <c r="N34" s="14"/>
       <c r="O34" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="P34" s="44"/>
+        <v>107</v>
+      </c>
+      <c r="P34" s="52"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="43" t="s">
-        <v>120</v>
+        <v>64</v>
+      </c>
+      <c r="E35" s="42" t="s">
+        <v>112</v>
       </c>
       <c r="F35" s="15">
         <v>43173</v>
@@ -2241,7 +2280,7 @@
         <v>37</v>
       </c>
       <c r="D37" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E37" s="16" t="s">
         <v>13</v>
@@ -2268,7 +2307,7 @@
       <c r="M37" s="2"/>
       <c r="N37" s="14"/>
       <c r="O37" s="40" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
@@ -2276,7 +2315,7 @@
         <v>38</v>
       </c>
       <c r="D38" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E38" s="16" t="s">
         <v>13</v>
@@ -2303,7 +2342,7 @@
       <c r="M38" s="40"/>
       <c r="N38" s="14"/>
       <c r="O38" s="40" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
@@ -2312,7 +2351,7 @@
       </c>
       <c r="C39" s="3"/>
       <c r="D39" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E39" s="16" t="s">
         <v>13</v>
@@ -2339,16 +2378,16 @@
       <c r="M39" s="2"/>
       <c r="N39" s="14"/>
       <c r="O39" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="P39" s="44"/>
+        <v>71</v>
+      </c>
+      <c r="P39" s="52"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="25">
         <v>40</v>
       </c>
       <c r="D40" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E40" s="16" t="s">
         <v>13</v>
@@ -2375,13 +2414,13 @@
       <c r="M40" s="2"/>
       <c r="N40" s="14"/>
       <c r="O40" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="P40" s="44"/>
+        <v>71</v>
+      </c>
+      <c r="P40" s="52"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E41" s="16" t="s">
         <v>13</v>
@@ -2408,12 +2447,12 @@
       <c r="M41" s="2"/>
       <c r="N41" s="14"/>
       <c r="O41" s="40" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E42" s="16" t="s">
         <v>13</v>
@@ -2440,7 +2479,7 @@
       <c r="M42" s="40"/>
       <c r="N42" s="14"/>
       <c r="O42" s="40" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
@@ -2513,7 +2552,7 @@
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" s="40" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
@@ -2539,9 +2578,9 @@
       <c r="M46" s="40"/>
       <c r="N46" s="2"/>
       <c r="O46" s="40" t="s">
-        <v>118</v>
-      </c>
-      <c r="P46" s="44"/>
+        <v>110</v>
+      </c>
+      <c r="P46" s="52"/>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E47" s="16" t="s">
@@ -2692,7 +2731,7 @@
         <v>57</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F55" s="15"/>
       <c r="G55" s="15"/>
@@ -2708,7 +2747,7 @@
         <v>58</v>
       </c>
       <c r="D56" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E56" s="16" t="s">
         <v>13</v>
@@ -2727,7 +2766,7 @@
         <v>43222</v>
       </c>
       <c r="K56" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -2738,7 +2777,7 @@
         <v>59</v>
       </c>
       <c r="D57" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E57" s="16" t="s">
         <v>13</v>
@@ -2762,7 +2801,7 @@
       <c r="M57" s="2"/>
       <c r="N57" s="40"/>
       <c r="O57" s="40" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.25">
@@ -2770,7 +2809,7 @@
         <v>60</v>
       </c>
       <c r="D58" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E58" s="16" t="s">
         <v>13</v>
@@ -2794,13 +2833,16 @@
       <c r="M58" s="40"/>
       <c r="N58" s="40"/>
       <c r="O58" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="P58" s="44"/>
+        <v>114</v>
+      </c>
+      <c r="P58" s="52"/>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B59" s="25">
+        <v>61</v>
+      </c>
       <c r="D59" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>13</v>
@@ -2824,137 +2866,208 @@
       <c r="M59" s="40"/>
       <c r="N59" s="40"/>
       <c r="O59" s="40" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
+      <c r="B60" s="25">
+        <v>62</v>
+      </c>
+      <c r="D60" t="s">
+        <v>77</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="15">
+        <v>43215</v>
+      </c>
+      <c r="G60" s="15">
+        <v>43222</v>
+      </c>
       <c r="H60" s="15"/>
-      <c r="I60" s="39"/>
-      <c r="J60" s="39"/>
+      <c r="I60" s="39">
+        <v>43215</v>
+      </c>
+      <c r="J60" s="39">
+        <v>43222</v>
+      </c>
+      <c r="K60" t="s">
+        <v>28</v>
+      </c>
       <c r="M60" s="40"/>
       <c r="N60" s="40"/>
-      <c r="O60" s="40"/>
+      <c r="O60" s="40" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B61" s="25">
-        <v>61</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D61" t="s">
-        <v>85</v>
-      </c>
-      <c r="E61" s="16" t="s">
-        <v>13</v>
-      </c>
       <c r="F61" s="15"/>
       <c r="G61" s="15"/>
       <c r="H61" s="15"/>
-      <c r="I61" s="39">
-        <v>43215</v>
-      </c>
-      <c r="J61" s="39">
-        <v>43222</v>
-      </c>
-      <c r="K61" t="s">
-        <v>28</v>
-      </c>
+      <c r="I61" s="39"/>
+      <c r="J61" s="39"/>
       <c r="M61" s="40"/>
       <c r="N61" s="40"/>
-      <c r="O61" s="40" t="s">
-        <v>85</v>
-      </c>
+      <c r="O61" s="40"/>
     </row>
     <row r="62" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B62" s="25">
         <v>62</v>
       </c>
-      <c r="D62" t="s">
-        <v>53</v>
-      </c>
-      <c r="E62" s="17"/>
-      <c r="F62" s="15">
-        <v>43222</v>
-      </c>
-      <c r="G62" s="15">
-        <v>43229</v>
-      </c>
+      <c r="C62" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
       <c r="H62" s="15"/>
-      <c r="M62" s="40"/>
-      <c r="N62" s="40"/>
-      <c r="O62" s="40"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+      <c r="O62" s="2"/>
     </row>
     <row r="63" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B63" s="25">
         <v>63</v>
       </c>
       <c r="D63" t="s">
-        <v>54</v>
-      </c>
-      <c r="E63" s="17"/>
+        <v>78</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="F63" s="15">
         <v>43222</v>
       </c>
       <c r="G63" s="15">
         <v>43229</v>
       </c>
-      <c r="H63" s="15"/>
+      <c r="H63" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I63" s="39">
+        <v>43222</v>
+      </c>
+      <c r="J63" s="39">
+        <v>43229</v>
+      </c>
+      <c r="K63" t="s">
+        <v>29</v>
+      </c>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
-      <c r="O63" s="2"/>
+      <c r="O63" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="P63" s="52"/>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B64" s="25">
         <v>64</v>
       </c>
       <c r="D64" t="s">
-        <v>55</v>
-      </c>
-      <c r="E64" s="17"/>
+        <v>79</v>
+      </c>
+      <c r="E64" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="F64" s="15">
         <v>43222</v>
       </c>
       <c r="G64" s="15">
         <v>43229</v>
       </c>
-      <c r="H64" s="15"/>
+      <c r="H64" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I64" s="39">
+        <v>43222</v>
+      </c>
+      <c r="J64" s="39">
+        <v>43229</v>
+      </c>
+      <c r="K64" t="s">
+        <v>28</v>
+      </c>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
-      <c r="O64" s="2"/>
-    </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="F65" s="15"/>
-      <c r="G65" s="15"/>
-      <c r="H65" s="15"/>
+      <c r="O64" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="P64" s="52"/>
+    </row>
+    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B65" s="25">
+        <v>65</v>
+      </c>
+      <c r="D65" t="s">
+        <v>80</v>
+      </c>
+      <c r="E65" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="15">
+        <v>43222</v>
+      </c>
+      <c r="G65" s="15">
+        <v>43229</v>
+      </c>
+      <c r="H65" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I65" s="39">
+        <v>43222</v>
+      </c>
+      <c r="J65" s="39">
+        <v>43229</v>
+      </c>
+      <c r="K65" t="s">
+        <v>109</v>
+      </c>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
       <c r="O65" s="2"/>
-    </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P65" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="2:16" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="25">
-        <v>65</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F66" s="15"/>
-      <c r="G66" s="15"/>
-      <c r="H66" s="15"/>
+        <v>66</v>
+      </c>
+      <c r="D66" t="s">
+        <v>81</v>
+      </c>
+      <c r="E66" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="F66" s="15">
+        <v>43222</v>
+      </c>
+      <c r="G66" s="15">
+        <v>43229</v>
+      </c>
+      <c r="H66" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I66" s="39"/>
+      <c r="J66" s="39"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
-    </row>
-    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P66" s="53" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B67" s="25">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D67" t="s">
-        <v>86</v>
-      </c>
-      <c r="E67" s="17"/>
+        <v>78</v>
+      </c>
+      <c r="E67" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="F67" s="15">
         <v>43222</v>
       </c>
@@ -2962,128 +3075,129 @@
         <v>43229</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>29</v>
+        <v>38</v>
+      </c>
+      <c r="I67" s="39">
+        <v>43222</v>
+      </c>
+      <c r="J67" s="39">
+        <v>43229</v>
+      </c>
+      <c r="K67" t="s">
+        <v>38</v>
       </c>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
       <c r="O67" s="40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="25">
-        <v>67</v>
-      </c>
-      <c r="D68" t="s">
-        <v>87</v>
-      </c>
-      <c r="E68" s="17"/>
-      <c r="F68" s="15">
-        <v>43222</v>
-      </c>
-      <c r="G68" s="15">
-        <v>43229</v>
-      </c>
-      <c r="H68" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="M68" s="2"/>
-      <c r="N68" s="2"/>
-      <c r="O68" s="2"/>
-    </row>
-    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="25">
-        <v>68</v>
-      </c>
-      <c r="D69" t="s">
-        <v>88</v>
-      </c>
-      <c r="E69" s="17"/>
-      <c r="F69" s="15">
-        <v>43222</v>
-      </c>
-      <c r="G69" s="15">
-        <v>43229</v>
-      </c>
-      <c r="H69" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="M69" s="2"/>
-      <c r="N69" s="2"/>
-      <c r="O69" s="2"/>
-    </row>
-    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="25">
-        <v>69</v>
-      </c>
-      <c r="D70" t="s">
-        <v>89</v>
-      </c>
-      <c r="F70" s="15">
-        <v>43222</v>
-      </c>
-      <c r="G70" s="15">
-        <v>43229</v>
-      </c>
-      <c r="H70" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
-        <v>86</v>
-      </c>
-      <c r="F71" s="15">
-        <v>43222</v>
-      </c>
-      <c r="G71" s="15">
-        <v>43229</v>
-      </c>
-      <c r="H71" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="O71" s="40" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C73" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="P67" s="52"/>
+    </row>
+    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I68" s="39"/>
+      <c r="J68" s="39"/>
+    </row>
+    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C69" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G69" s="39"/>
+    </row>
+    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>54</v>
+      </c>
+      <c r="D70" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="E70" s="52"/>
+      <c r="F70" s="52"/>
+    </row>
+    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>56</v>
+      </c>
+      <c r="D71" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="G73" s="39"/>
-    </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E71" s="54"/>
+      <c r="F71" s="54"/>
+      <c r="G71" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="72" spans="2:16" ht="105" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>58</v>
+      </c>
+      <c r="D72" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E72" s="43"/>
+      <c r="F72" s="43"/>
+      <c r="G72" s="53" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>123</v>
+      </c>
+      <c r="D73" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="E73" s="52"/>
+      <c r="F73" s="52"/>
+    </row>
+    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>58</v>
+        <v>124</v>
       </c>
       <c r="D74" s="41" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="E74" s="54"/>
+      <c r="F74" s="54"/>
+      <c r="G74" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="D75" s="41" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="E75" s="52"/>
+      <c r="F75" s="52"/>
+    </row>
+    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>62</v>
+        <v>132</v>
       </c>
       <c r="D76" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="E76" s="44"/>
-      <c r="F76" s="44"/>
-    </row>
-    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C77" s="42" t="s">
-        <v>80</v>
+        <v>113</v>
+      </c>
+      <c r="E76" s="52"/>
+      <c r="F76" s="52"/>
+    </row>
+    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>133</v>
       </c>
       <c r="D77" s="41" t="s">
-        <v>81</v>
+        <v>128</v>
+      </c>
+      <c r="E77" s="52"/>
+      <c r="F77" s="52"/>
+    </row>
+    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>134</v>
+      </c>
+      <c r="D78" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -3101,7 +3215,7 @@
   <hyperlinks>
     <hyperlink ref="O10" r:id="rId1" display="1-Gauthier-Levitation"/>
     <hyperlink ref="O11" r:id="rId2" display="1-Satish-RcCars"/>
-    <hyperlink ref="O12" r:id="rId3" display="1-Ali-SmartRoom"/>
+    <hyperlink ref="O12" r:id="rId3"/>
     <hyperlink ref="O13" r:id="rId4" display="1-Daniel-RFID"/>
     <hyperlink ref="O18" r:id="rId5" display="2-Gauthier-NodeMCU"/>
     <hyperlink ref="O19" r:id="rId6" display="2-Satish-Car"/>
@@ -3112,34 +3226,38 @@
     <hyperlink ref="O26" r:id="rId11" display="3_Satish_RCCarVsOtherCars"/>
     <hyperlink ref="O27" r:id="rId12" display="3_Asif_Server_OS_comparison"/>
     <hyperlink ref="O28" r:id="rId13" display="3_Gauthier_Different-Microcontrollers"/>
-    <hyperlink ref="O25" r:id="rId14" display="3_Ali_NodeMCU-programming"/>
+    <hyperlink ref="O25" r:id="rId14"/>
     <hyperlink ref="N27" r:id="rId15"/>
     <hyperlink ref="O31" r:id="rId16" display="4 Asif Server_connection_nodeMCU"/>
     <hyperlink ref="O32" r:id="rId17" display="4 Daniel WP_Motor_Programming"/>
     <hyperlink ref="O33" r:id="rId18" display="4 Gauthier21_03 ESP8266 Programming"/>
-    <hyperlink ref="O34" r:id="rId19" display="4 Ali NodeMCU-UDP"/>
+    <hyperlink ref="O34" r:id="rId19"/>
     <hyperlink ref="O37" r:id="rId20" display="5-Asif Measuring UDP latency"/>
     <hyperlink ref="O38" r:id="rId21" display="5-Gauthier sonar ranging module"/>
     <hyperlink ref="O39" r:id="rId22"/>
-    <hyperlink ref="O40" r:id="rId23"/>
-    <hyperlink ref="O41" r:id="rId24"/>
-    <hyperlink ref="O42" r:id="rId25" display="5-WP_Motor_Programming_Daniel_SmetankinV2"/>
-    <hyperlink ref="O46" r:id="rId26"/>
-    <hyperlink ref="O45" r:id="rId27"/>
-    <hyperlink ref="O58" r:id="rId28"/>
-    <hyperlink ref="O59" r:id="rId29"/>
-    <hyperlink ref="O61" r:id="rId30"/>
-    <hyperlink ref="D74" r:id="rId31"/>
-    <hyperlink ref="D75" r:id="rId32"/>
-    <hyperlink ref="D76" r:id="rId33"/>
-    <hyperlink ref="D77" r:id="rId34"/>
-    <hyperlink ref="O57" r:id="rId35"/>
-    <hyperlink ref="O67" r:id="rId36"/>
-    <hyperlink ref="O71" r:id="rId37"/>
+    <hyperlink ref="O41" r:id="rId23"/>
+    <hyperlink ref="O42" r:id="rId24" display="5-WP_Motor_Programming_Daniel_SmetankinV2"/>
+    <hyperlink ref="O46" r:id="rId25"/>
+    <hyperlink ref="O45" r:id="rId26"/>
+    <hyperlink ref="O58" r:id="rId27"/>
+    <hyperlink ref="O59" r:id="rId28" display="SoftwareUpdates"/>
+    <hyperlink ref="O60" r:id="rId29" display="Inrushcurrent"/>
+    <hyperlink ref="D70" r:id="rId30"/>
+    <hyperlink ref="D71" r:id="rId31"/>
+    <hyperlink ref="D72" r:id="rId32"/>
+    <hyperlink ref="D76" r:id="rId33" display="Report9"/>
+    <hyperlink ref="O57" r:id="rId34" display="Poster+ideaFormulation"/>
+    <hyperlink ref="O63" r:id="rId35" display="7-Gauthier de Borrekens_poster_ideas"/>
+    <hyperlink ref="O67" r:id="rId36" display="7-Asif Wasefi_poster_ideas"/>
+    <hyperlink ref="D77" r:id="rId37" display="Report7"/>
+    <hyperlink ref="O40" r:id="rId38"/>
+    <hyperlink ref="O64" r:id="rId39"/>
+    <hyperlink ref="D73" r:id="rId40"/>
+    <hyperlink ref="D75" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
-  <legacyDrawing r:id="rId39"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
+  <legacyDrawing r:id="rId43"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
uploaded preparation and updated project report
</commit_message>
<xml_diff>
--- a/SP_2018_03_06_CarToCarCommunicationRECENTST.xlsx
+++ b/SP_2018_03_06_CarToCarCommunicationRECENTST.xlsx
@@ -1310,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>